<commit_message>
Corrección de documentos, entrega final.
</commit_message>
<xml_diff>
--- a/Fase 1/DocumentosProyecto/Carta Gantt OfCourse.xlsx
+++ b/Fase 1/DocumentosProyecto/Carta Gantt OfCourse.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="Fngfg7/wkEav8cof7cpGsgDHUn6xzuggyaTpnmUCoNQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="v1VqkaDJHgk67wRadFbOkrqprQfVMJ6srRH52m3YhWw="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Proyecto : DuocOfCourse</t>
   </si>
@@ -108,7 +108,7 @@
     <t>Modelamiento BD</t>
   </si>
   <si>
-    <t>Desarrollo frontend</t>
+    <t>Desarrollo frontend sistema web</t>
   </si>
   <si>
     <t>Entrega Modelo arquitectonico</t>
@@ -117,10 +117,13 @@
     <t>Desarrollo BD</t>
   </si>
   <si>
-    <t>Desarrollo Backend</t>
+    <t>Desarrollo Backend sistema web</t>
   </si>
   <si>
     <t>Implementación de APIs</t>
+  </si>
+  <si>
+    <t>Desarrollo sistema de escritorio</t>
   </si>
   <si>
     <t>Entrega 100% desarrollo</t>
@@ -145,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -162,6 +165,11 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -260,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -286,6 +294,9 @@
     <xf borderId="7" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,32 +707,32 @@
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="11" t="s">
+    <row r="19">
+      <c r="A19" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="T19" s="12"/>
+      <c r="S19" s="12"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
+      <c r="T20" s="12"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="U21" s="12"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="V22" s="12"/>
+      <c r="U22" s="12"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="13" t="s">
@@ -733,10 +744,17 @@
       <c r="A24" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="W24" s="12"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
+      <c r="V24" s="12"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="W25" s="12"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="B26" s="14"/>
+    </row>
     <row r="27" ht="15.75" customHeight="1"/>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1"/>
@@ -1709,15 +1727,16 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="L4:T4"/>
     <mergeCell ref="U4:W4"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A8:E8"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="F4:K4"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:E11"/>
@@ -1725,15 +1744,16 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A22:E22"/>
     <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>